<commit_message>
Correction et ajout paragraphe gestion id 05433b429643ad4012f3907179b7d8f364525991
</commit_message>
<xml_diff>
--- a/346-flux---gestion-des-ids/ig/StructureDefinition-tddui-bundle.xlsx
+++ b/346-flux---gestion-des-ids/ig/StructureDefinition-tddui-bundle.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-08-22T13:38:23+00:00</t>
+    <t>2025-09-12T07:57:25+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -361,7 +361,7 @@
     <t>A human language.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/languages</t>
+    <t>http://hl7.org/fhir/ValueSet/languages|4.0.1</t>
   </si>
   <si>
     <t>Resource.language</t>

</xml_diff>